<commit_message>
chore: publish homecareobservation IG 1.1.1-trial-use
</commit_message>
<xml_diff>
--- a/ig/homecareobservation/StructureDefinition-medcom-homecare-observation.xlsx
+++ b/ig/homecareobservation/StructureDefinition-medcom-homecare-observation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7819" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7819" uniqueCount="748">
   <si>
     <t>Property</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0-trial-use</t>
+    <t>1.1.1-trial-use</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-08T10:47:31+00:00</t>
+    <t>2025-09-17T12:02:53+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1293,7 +1293,7 @@
   </si>
   <si>
     <t>Quantity
-string</t>
+CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
   </si>
   <si>
     <t>Actual result</t>
@@ -2242,10 +2242,6 @@
   </si>
   <si>
     <t>Observation.component.value[x]</t>
-  </si>
-  <si>
-    <t>Quantity
-CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
   </si>
   <si>
     <t>Actual component result</t>
@@ -25772,16 +25768,16 @@
         <v>94</v>
       </c>
       <c r="K192" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="L192" t="s" s="2">
         <v>720</v>
-      </c>
-      <c r="L192" t="s" s="2">
-        <v>721</v>
       </c>
       <c r="M192" t="s" s="2">
         <v>414</v>
       </c>
       <c r="N192" t="s" s="2">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="O192" t="s" s="2">
         <v>416</v>
@@ -25849,7 +25845,7 @@
         <v>82</v>
       </c>
       <c r="AL192" t="s" s="2">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="AM192" t="s" s="2">
         <v>420</v>
@@ -25866,7 +25862,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B193" t="s" s="2">
         <v>719</v>
@@ -25897,13 +25893,13 @@
         <v>425</v>
       </c>
       <c r="L193" t="s" s="2">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="M193" t="s" s="2">
         <v>414</v>
       </c>
       <c r="N193" t="s" s="2">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="O193" t="s" s="2">
         <v>416</v>
@@ -25973,7 +25969,7 @@
         <v>82</v>
       </c>
       <c r="AL193" t="s" s="2">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="AM193" t="s" s="2">
         <v>420</v>
@@ -25990,10 +25986,10 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
+        <v>724</v>
+      </c>
+      <c r="B194" t="s" s="2">
         <v>725</v>
-      </c>
-      <c r="B194" t="s" s="2">
-        <v>726</v>
       </c>
       <c r="C194" s="2"/>
       <c r="D194" t="s" s="2">
@@ -26108,10 +26104,10 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
+        <v>726</v>
+      </c>
+      <c r="B195" t="s" s="2">
         <v>727</v>
-      </c>
-      <c r="B195" t="s" s="2">
-        <v>728</v>
       </c>
       <c r="C195" s="2"/>
       <c r="D195" t="s" s="2">
@@ -26228,10 +26224,10 @@
     </row>
     <row r="196" hidden="true">
       <c r="A196" t="s" s="2">
+        <v>728</v>
+      </c>
+      <c r="B196" t="s" s="2">
         <v>729</v>
-      </c>
-      <c r="B196" t="s" s="2">
-        <v>730</v>
       </c>
       <c r="C196" s="2"/>
       <c r="D196" t="s" s="2">
@@ -26350,10 +26346,10 @@
     </row>
     <row r="197" hidden="true">
       <c r="A197" t="s" s="2">
+        <v>730</v>
+      </c>
+      <c r="B197" t="s" s="2">
         <v>731</v>
-      </c>
-      <c r="B197" t="s" s="2">
-        <v>732</v>
       </c>
       <c r="C197" s="2"/>
       <c r="D197" t="s" s="2">
@@ -26472,10 +26468,10 @@
     </row>
     <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
+        <v>732</v>
+      </c>
+      <c r="B198" t="s" s="2">
         <v>733</v>
-      </c>
-      <c r="B198" t="s" s="2">
-        <v>734</v>
       </c>
       <c r="C198" s="2"/>
       <c r="D198" t="s" s="2">
@@ -26592,10 +26588,10 @@
     </row>
     <row r="199" hidden="true">
       <c r="A199" t="s" s="2">
+        <v>734</v>
+      </c>
+      <c r="B199" t="s" s="2">
         <v>735</v>
-      </c>
-      <c r="B199" t="s" s="2">
-        <v>736</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" t="s" s="2">
@@ -26712,10 +26708,10 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
+        <v>736</v>
+      </c>
+      <c r="B200" t="s" s="2">
         <v>737</v>
-      </c>
-      <c r="B200" t="s" s="2">
-        <v>738</v>
       </c>
       <c r="C200" s="2"/>
       <c r="D200" t="s" s="2">
@@ -26834,10 +26830,10 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B201" t="s" s="2">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C201" s="2"/>
       <c r="D201" t="s" s="2">
@@ -26863,13 +26859,13 @@
         <v>190</v>
       </c>
       <c r="L201" t="s" s="2">
+        <v>739</v>
+      </c>
+      <c r="M201" t="s" s="2">
         <v>740</v>
       </c>
-      <c r="M201" t="s" s="2">
+      <c r="N201" t="s" s="2">
         <v>741</v>
-      </c>
-      <c r="N201" t="s" s="2">
-        <v>742</v>
       </c>
       <c r="O201" t="s" s="2">
         <v>483</v>
@@ -26921,7 +26917,7 @@
         <v>82</v>
       </c>
       <c r="AF201" t="s" s="2">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="AG201" t="s" s="2">
         <v>80</v>
@@ -26956,10 +26952,10 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B202" t="s" s="2">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C202" s="2"/>
       <c r="D202" t="s" s="2">
@@ -27022,11 +27018,11 @@
         <v>484</v>
       </c>
       <c r="Y202" t="s" s="2">
+        <v>743</v>
+      </c>
+      <c r="Z202" t="s" s="2">
         <v>744</v>
       </c>
-      <c r="Z202" t="s" s="2">
-        <v>745</v>
-      </c>
       <c r="AA202" t="s" s="2">
         <v>82</v>
       </c>
@@ -27043,7 +27039,7 @@
         <v>82</v>
       </c>
       <c r="AF202" t="s" s="2">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="AG202" t="s" s="2">
         <v>80</v>
@@ -27078,10 +27074,10 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B203" t="s" s="2">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C203" s="2"/>
       <c r="D203" t="s" s="2">
@@ -27107,10 +27103,10 @@
         <v>83</v>
       </c>
       <c r="L203" t="s" s="2">
+        <v>746</v>
+      </c>
+      <c r="M203" t="s" s="2">
         <v>747</v>
-      </c>
-      <c r="M203" t="s" s="2">
-        <v>748</v>
       </c>
       <c r="N203" t="s" s="2">
         <v>582</v>
@@ -27165,7 +27161,7 @@
         <v>82</v>
       </c>
       <c r="AF203" t="s" s="2">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AG203" t="s" s="2">
         <v>80</v>

</xml_diff>

<commit_message>
chore: publish homecareobservation IG 1.1.1-trial-use (#32)
Co-authored-by: olw-medcom <olw-medcom@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ig/homecareobservation/StructureDefinition-medcom-homecare-observation.xlsx
+++ b/ig/homecareobservation/StructureDefinition-medcom-homecare-observation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7819" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7819" uniqueCount="748">
   <si>
     <t>Property</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0-trial-use</t>
+    <t>1.1.1-trial-use</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-08T10:47:31+00:00</t>
+    <t>2025-09-17T12:02:53+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1293,7 +1293,7 @@
   </si>
   <si>
     <t>Quantity
-string</t>
+CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
   </si>
   <si>
     <t>Actual result</t>
@@ -2242,10 +2242,6 @@
   </si>
   <si>
     <t>Observation.component.value[x]</t>
-  </si>
-  <si>
-    <t>Quantity
-CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
   </si>
   <si>
     <t>Actual component result</t>
@@ -25772,16 +25768,16 @@
         <v>94</v>
       </c>
       <c r="K192" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="L192" t="s" s="2">
         <v>720</v>
-      </c>
-      <c r="L192" t="s" s="2">
-        <v>721</v>
       </c>
       <c r="M192" t="s" s="2">
         <v>414</v>
       </c>
       <c r="N192" t="s" s="2">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="O192" t="s" s="2">
         <v>416</v>
@@ -25849,7 +25845,7 @@
         <v>82</v>
       </c>
       <c r="AL192" t="s" s="2">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="AM192" t="s" s="2">
         <v>420</v>
@@ -25866,7 +25862,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B193" t="s" s="2">
         <v>719</v>
@@ -25897,13 +25893,13 @@
         <v>425</v>
       </c>
       <c r="L193" t="s" s="2">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="M193" t="s" s="2">
         <v>414</v>
       </c>
       <c r="N193" t="s" s="2">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="O193" t="s" s="2">
         <v>416</v>
@@ -25973,7 +25969,7 @@
         <v>82</v>
       </c>
       <c r="AL193" t="s" s="2">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="AM193" t="s" s="2">
         <v>420</v>
@@ -25990,10 +25986,10 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
+        <v>724</v>
+      </c>
+      <c r="B194" t="s" s="2">
         <v>725</v>
-      </c>
-      <c r="B194" t="s" s="2">
-        <v>726</v>
       </c>
       <c r="C194" s="2"/>
       <c r="D194" t="s" s="2">
@@ -26108,10 +26104,10 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
+        <v>726</v>
+      </c>
+      <c r="B195" t="s" s="2">
         <v>727</v>
-      </c>
-      <c r="B195" t="s" s="2">
-        <v>728</v>
       </c>
       <c r="C195" s="2"/>
       <c r="D195" t="s" s="2">
@@ -26228,10 +26224,10 @@
     </row>
     <row r="196" hidden="true">
       <c r="A196" t="s" s="2">
+        <v>728</v>
+      </c>
+      <c r="B196" t="s" s="2">
         <v>729</v>
-      </c>
-      <c r="B196" t="s" s="2">
-        <v>730</v>
       </c>
       <c r="C196" s="2"/>
       <c r="D196" t="s" s="2">
@@ -26350,10 +26346,10 @@
     </row>
     <row r="197" hidden="true">
       <c r="A197" t="s" s="2">
+        <v>730</v>
+      </c>
+      <c r="B197" t="s" s="2">
         <v>731</v>
-      </c>
-      <c r="B197" t="s" s="2">
-        <v>732</v>
       </c>
       <c r="C197" s="2"/>
       <c r="D197" t="s" s="2">
@@ -26472,10 +26468,10 @@
     </row>
     <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
+        <v>732</v>
+      </c>
+      <c r="B198" t="s" s="2">
         <v>733</v>
-      </c>
-      <c r="B198" t="s" s="2">
-        <v>734</v>
       </c>
       <c r="C198" s="2"/>
       <c r="D198" t="s" s="2">
@@ -26592,10 +26588,10 @@
     </row>
     <row r="199" hidden="true">
       <c r="A199" t="s" s="2">
+        <v>734</v>
+      </c>
+      <c r="B199" t="s" s="2">
         <v>735</v>
-      </c>
-      <c r="B199" t="s" s="2">
-        <v>736</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" t="s" s="2">
@@ -26712,10 +26708,10 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
+        <v>736</v>
+      </c>
+      <c r="B200" t="s" s="2">
         <v>737</v>
-      </c>
-      <c r="B200" t="s" s="2">
-        <v>738</v>
       </c>
       <c r="C200" s="2"/>
       <c r="D200" t="s" s="2">
@@ -26834,10 +26830,10 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B201" t="s" s="2">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C201" s="2"/>
       <c r="D201" t="s" s="2">
@@ -26863,13 +26859,13 @@
         <v>190</v>
       </c>
       <c r="L201" t="s" s="2">
+        <v>739</v>
+      </c>
+      <c r="M201" t="s" s="2">
         <v>740</v>
       </c>
-      <c r="M201" t="s" s="2">
+      <c r="N201" t="s" s="2">
         <v>741</v>
-      </c>
-      <c r="N201" t="s" s="2">
-        <v>742</v>
       </c>
       <c r="O201" t="s" s="2">
         <v>483</v>
@@ -26921,7 +26917,7 @@
         <v>82</v>
       </c>
       <c r="AF201" t="s" s="2">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="AG201" t="s" s="2">
         <v>80</v>
@@ -26956,10 +26952,10 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B202" t="s" s="2">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C202" s="2"/>
       <c r="D202" t="s" s="2">
@@ -27022,11 +27018,11 @@
         <v>484</v>
       </c>
       <c r="Y202" t="s" s="2">
+        <v>743</v>
+      </c>
+      <c r="Z202" t="s" s="2">
         <v>744</v>
       </c>
-      <c r="Z202" t="s" s="2">
-        <v>745</v>
-      </c>
       <c r="AA202" t="s" s="2">
         <v>82</v>
       </c>
@@ -27043,7 +27039,7 @@
         <v>82</v>
       </c>
       <c r="AF202" t="s" s="2">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="AG202" t="s" s="2">
         <v>80</v>
@@ -27078,10 +27074,10 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B203" t="s" s="2">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C203" s="2"/>
       <c r="D203" t="s" s="2">
@@ -27107,10 +27103,10 @@
         <v>83</v>
       </c>
       <c r="L203" t="s" s="2">
+        <v>746</v>
+      </c>
+      <c r="M203" t="s" s="2">
         <v>747</v>
-      </c>
-      <c r="M203" t="s" s="2">
-        <v>748</v>
       </c>
       <c r="N203" t="s" s="2">
         <v>582</v>
@@ -27165,7 +27161,7 @@
         <v>82</v>
       </c>
       <c r="AF203" t="s" s="2">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AG203" t="s" s="2">
         <v>80</v>

</xml_diff>

<commit_message>
chore: publish homecareobservation IG 1.2.1
</commit_message>
<xml_diff>
--- a/ig/homecareobservation/StructureDefinition-medcom-homecare-observation.xlsx
+++ b/ig/homecareobservation/StructureDefinition-medcom-homecare-observation.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.2.0</t>
+    <t>1.2.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-03T12:37:39+00:00</t>
+    <t>2025-12-19T07:53:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
chore: publish homecareobservation IG 1.2.1 (#56)
Co-authored-by: olw-medcom <olw-medcom@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ig/homecareobservation/StructureDefinition-medcom-homecare-observation.xlsx
+++ b/ig/homecareobservation/StructureDefinition-medcom-homecare-observation.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.2.0</t>
+    <t>1.2.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-03T12:37:39+00:00</t>
+    <t>2025-12-19T07:53:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>